<commit_message>
Fix sur la selection et visualisation des campagnes
</commit_message>
<xml_diff>
--- a/data/Upload/Session/1/Campagne_1.xlsx
+++ b/data/Upload/Session/1/Campagne_1.xlsx
@@ -15,63 +15,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
-    <t>George</t>
+    <t>Participant</t>
   </si>
   <si>
-    <t>1:1, 1:2, 2:2, 3:2, 2:3</t>
+    <t>1:1, 2:2, 2:3, 3:3, 3:2, 4:2, 3:1, 4:1, 3:4, 2:3, 2:4, 1:3, 1:4, 2:2</t>
   </si>
   <si>
-    <t>Prodit 3, Prodit 4, Prodit 4, Prodit 4, Prodit 2</t>
+    <t>Prodit A, prodit C, prodit B, prodit B, prodit C, prodit C, Prodit A, Prodit A, prodit C, prodit B, prodit C, prodit B, prodit C, prodit C</t>
   </si>
   <si>
-    <t>Lettre, Lettre, Chiffre, Mot, Chiffre</t>
+    <t>Prodit \xe9qitable, "Pr\xe9sence dn label", "Pr\xe9sence dn label", prodit drable, prodit drable, Prodit bio, prodit drable, Prodit bio, prodit drable, "Pr\xe9sence dn label", "Pr\xe9sence dn label", Prodit \xe9qitable, Prodit \xe9qitable, "Pr\xe9sence dn label"</t>
   </si>
   <si>
-    <t>Produit 2</t>
-  </si>
-  <si>
-    <t>Produit 4</t>
-  </si>
-  <si>
-    <t>2:2, 1:1, 1:2, 2:3, 3:3, 3:4, 2:4, 3:2, 3:1, 1:2, 1:4</t>
-  </si>
-  <si>
-    <t>Prodit 4, Prodit 3, Prodit 4, Prodit 2, Prodit 2, Prodit 1, Prodit 1, Prodit 4, Prodit 3, Prodit 4, Prodit 1</t>
-  </si>
-  <si>
-    <t>Mot, Chiffre, Chiffre, Mot, Lettre, Lettre, Mot, Lettre, Lettre, Chiffre, Chiffre</t>
-  </si>
-  <si>
-    <t>Produit 1</t>
-  </si>
-  <si>
-    <t>1:1, 1:2, 2:2, 2:3, 3:3, 2:4</t>
-  </si>
-  <si>
-    <t>Prodit 1, Prodit 4, Prodit 4, Prodit 3, Prodit 3, Prodit 2</t>
-  </si>
-  <si>
-    <t>Lettre, Lettre, Chiffre, Chiffre, Mot, Chiffre</t>
-  </si>
-  <si>
-    <t>2:1, 2:2, 1:3, 2:3, 3:3, 3:4, 1:2</t>
-  </si>
-  <si>
-    <t>Prodit 3, Prodit 4, Prodit 1, Prodit 1, Prodit 1, Prodit 2, Prodit 4</t>
-  </si>
-  <si>
-    <t>Chiffre, Chiffre, Mot, Chiffre, Lettre, Lettre, Mot</t>
-  </si>
-  <si>
-    <t>3:1, 2:2, 1:1, 2:1, 2:3, 1:3</t>
-  </si>
-  <si>
-    <t>Prodit 1, Prodit 4, Prodit 1, Prodit 1, Prodit 3, Prodit 3</t>
-  </si>
-  <si>
-    <t>Mot, Lettre, Chiffre, Lettre, Lettre, Chiffre</t>
+    <t>produit C</t>
   </si>
 </sst>
 </file>
@@ -407,7 +365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,200 +396,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s"/>
-      <c r="C2" t="s"/>
-      <c r="D2" t="s"/>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout du formulaire google dans la session du participant : identification du participant par token
</commit_message>
<xml_diff>
--- a/data/Upload/Session/1/Campagne_1.xlsx
+++ b/data/Upload/Session/1/Campagne_1.xlsx
@@ -17,19 +17,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
-    <t>Participant</t>
+    <t>C1IDc8d501</t>
   </si>
   <si>
-    <t>1:1, 2:2, 2:3, 3:3, 3:2, 4:2, 3:1, 4:1, 3:4, 2:3, 2:4, 1:3, 1:4, 2:2</t>
+    <t>1:1, 2:2, 3:2, 3:3, 4:3, 4:4, 3:4, 2:4, 1:4, 1:3</t>
   </si>
   <si>
-    <t>Prodit A, prodit C, prodit B, prodit B, prodit C, prodit C, Prodit A, Prodit A, prodit C, prodit B, prodit C, prodit B, prodit C, prodit C</t>
+    <t>Shining, Bles brothers, Bles brothers, 12 hommes en coleres, 12 hommes en coleres, Hellraiser, Hellraiser, Hellraiser, Hellraiser, 12 hommes en coleres</t>
   </si>
   <si>
-    <t>Prodit \xe9qitable, "Pr\xe9sence dn label", "Pr\xe9sence dn label", prodit drable, prodit drable, Prodit bio, prodit drable, Prodit bio, prodit drable, "Pr\xe9sence dn label", "Pr\xe9sence dn label", Prodit \xe9qitable, Prodit \xe9qitable, "Pr\xe9sence dn label"</t>
+    <t>Affiche, R\xe9alisater, Ann\xe9e, Ann\xe9e, Genre, Genre, Ann\xe9e, R\xe9alisater, Affiche, Affiche</t>
   </si>
   <si>
-    <t>produit C</t>
+    <t>12 hommes en coleres</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Fix du téléchargement des toutes les sessions
</commit_message>
<xml_diff>
--- a/data/Upload/Session/1/Campagne_1.xlsx
+++ b/data/Upload/Session/1/Campagne_1.xlsx
@@ -15,21 +15,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
-  <si>
-    <t>C1IDc8d501</t>
-  </si>
-  <si>
-    <t>1:1, 2:2, 3:2, 3:3, 4:3, 4:4, 3:4, 2:4, 1:4, 1:3</t>
-  </si>
-  <si>
-    <t>Shining, Bles brothers, Bles brothers, 12 hommes en coleres, 12 hommes en coleres, Hellraiser, Hellraiser, Hellraiser, Hellraiser, 12 hommes en coleres</t>
-  </si>
-  <si>
-    <t>Affiche, R\xe9alisater, Ann\xe9e, Ann\xe9e, Genre, Genre, Ann\xe9e, R\xe9alisater, Affiche, Affiche</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>Coords</t>
+  </si>
+  <si>
+    <t>Association Ligne</t>
+  </si>
+  <si>
+    <t>Association Col</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
+  </si>
+  <si>
+    <t>Temps total</t>
+  </si>
+  <si>
+    <t>Choix Final</t>
+  </si>
+  <si>
+    <t>Id Campagne</t>
+  </si>
+  <si>
+    <t>C1ID431991</t>
+  </si>
+  <si>
+    <t>2:1', 3:2', 3:3', 4:3', 4:4', 3:5'</t>
+  </si>
+  <si>
+    <t>Shining', Blues brothers', Hellraiser', Hellraiser', 12 hommes en coleres', Massacre \xe0 la tron\xe7onneuse'</t>
+  </si>
+  <si>
+    <t>R\xe9alisateur', Ann\xe9e', Ann\xe9e', Genre', Genre', Ann\xe9e'</t>
+  </si>
+  <si>
+    <t>Massacre à la tronçonneuse</t>
+  </si>
+  <si>
+    <t>C1IDe1f63e</t>
+  </si>
+  <si>
+    <t>2:1', 2:2', 3:3', 3:4', 1:5'</t>
+  </si>
+  <si>
+    <t>Hellraiser', Blues brothers', Massacre \xe0 la tron\xe7onneuse', Shining', 12 hommes en coleres'</t>
+  </si>
+  <si>
+    <t>R\xe9alisateur', R\xe9alisateur', Ann\xe9e', Ann\xe9e', Affiche'</t>
   </si>
   <si>
     <t>12 hommes en coleres</t>
+  </si>
+  <si>
+    <t>C1ID7f262d</t>
+  </si>
+  <si>
+    <t>2:1', 2:2', 2:3', 2:4', 2:5'</t>
+  </si>
+  <si>
+    <t>Massacre \xe0 la tron\xe7onneuse', Shining', 12 hommes en coleres', Hellraiser', Blues brothers'</t>
+  </si>
+  <si>
+    <t>Ann\xe9e', Ann\xe9e', Ann\xe9e', Ann\xe9e', Ann\xe9e'</t>
+  </si>
+  <si>
+    <t>Blues brothers</t>
   </si>
 </sst>
 </file>
@@ -37,13 +91,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +119,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -365,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -373,28 +440,169 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="n">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="n">
         <v>1</v>
       </c>
+      <c r="G2" t="n">
+        <v>3771</v>
+      </c>
+      <c r="H2" t="s"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3784</v>
+      </c>
+      <c r="H3" t="s"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2827</v>
+      </c>
+      <c r="H4" t="s"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s"/>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s"/>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s"/>
+      <c r="H5" t="s"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s"/>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s"/>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s"/>
+      <c r="H6" t="s"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s"/>
+      <c r="B7" t="s"/>
+      <c r="C7" t="s"/>
+      <c r="D7" t="s"/>
+      <c r="E7" t="s"/>
+      <c r="F7" t="s"/>
+      <c r="G7" t="s"/>
+      <c r="H7" t="s"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s"/>
+      <c r="B8" t="s"/>
+      <c r="C8" t="s"/>
+      <c r="D8" t="s"/>
+      <c r="E8" t="s"/>
+      <c r="F8" t="s"/>
+      <c r="G8" t="s"/>
+      <c r="H8" t="s"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s"/>
+      <c r="B9" t="s"/>
+      <c r="C9" t="s"/>
+      <c r="D9" t="s"/>
+      <c r="E9" t="s"/>
+      <c r="F9" t="s"/>
+      <c r="G9" t="s"/>
+      <c r="H9" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Ajout d'un systeme d'authentification, pour garentir une relative sécuritée
</commit_message>
<xml_diff>
--- a/data/Upload/Session/1/Campagne_1.xlsx
+++ b/data/Upload/Session/1/Campagne_1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Token</t>
   </si>
@@ -41,49 +41,19 @@
     <t>Id Campagne</t>
   </si>
   <si>
-    <t>C1ID431991</t>
-  </si>
-  <si>
-    <t>2:1', 3:2', 3:3', 4:3', 4:4', 3:5'</t>
-  </si>
-  <si>
-    <t>Shining', Blues brothers', Hellraiser', Hellraiser', 12 hommes en coleres', Massacre \xe0 la tron\xe7onneuse'</t>
-  </si>
-  <si>
-    <t>R\xe9alisateur', Ann\xe9e', Ann\xe9e', Genre', Genre', Ann\xe9e'</t>
-  </si>
-  <si>
-    <t>Massacre à la tronçonneuse</t>
-  </si>
-  <si>
-    <t>C1IDe1f63e</t>
-  </si>
-  <si>
-    <t>2:1', 2:2', 3:3', 3:4', 1:5'</t>
-  </si>
-  <si>
-    <t>Hellraiser', Blues brothers', Massacre \xe0 la tron\xe7onneuse', Shining', 12 hommes en coleres'</t>
-  </si>
-  <si>
-    <t>R\xe9alisateur', R\xe9alisateur', Ann\xe9e', Ann\xe9e', Affiche'</t>
-  </si>
-  <si>
-    <t>12 hommes en coleres</t>
-  </si>
-  <si>
-    <t>C1ID7f262d</t>
-  </si>
-  <si>
-    <t>2:1', 2:2', 2:3', 2:4', 2:5'</t>
-  </si>
-  <si>
-    <t>Massacre \xe0 la tron\xe7onneuse', Shining', 12 hommes en coleres', Hellraiser', Blues brothers'</t>
-  </si>
-  <si>
-    <t>Ann\xe9e', Ann\xe9e', Ann\xe9e', Ann\xe9e', Ann\xe9e'</t>
-  </si>
-  <si>
-    <t>Blues brothers</t>
+    <t>C1IDacb615</t>
+  </si>
+  <si>
+    <t>1:1', 2:2', 2:3', 3:3', 3:2', 4:2', 4:3', 4:4', 3:4', 4:1', 3:1', 2:3', 2:4', 1:4'</t>
+  </si>
+  <si>
+    <t>produit B', produit C', produit C', produit C', produit C', produit C', produit C', Produit A', Produit A', produit B', produit B', produit C', Produit A', Produit A'</t>
+  </si>
+  <si>
+    <t>u"Pr\xe9sence d'un label", produit durable', produit durable', Produit \xe9quitable', Produit \xe9quitable', Produit bio', Produit bio', Produit bio', Produit \xe9quitable', Produit bio', Produit \xe9quitable', produit durable', produit durable', u"Pr\xe9sence d'un label"</t>
+  </si>
+  <si>
+    <t>Produit A</t>
   </si>
 </sst>
 </file>
@@ -479,98 +449,56 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="n">
+        <v>560.8571428571429</v>
+      </c>
+      <c r="F2" t="n">
+        <v>7852</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" t="n">
-        <v>3771</v>
-      </c>
-      <c r="H2" t="s"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>3784</v>
-      </c>
+      <c r="A3" t="s"/>
+      <c r="B3" t="s"/>
+      <c r="C3" t="s"/>
+      <c r="D3" t="s"/>
+      <c r="E3" t="s"/>
+      <c r="F3" t="s"/>
+      <c r="G3" t="s"/>
       <c r="H3" t="s"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>2827</v>
-      </c>
+      <c r="A4" t="s"/>
+      <c r="B4" t="s"/>
+      <c r="C4" t="s"/>
+      <c r="D4" t="s"/>
+      <c r="E4" t="s"/>
+      <c r="F4" t="s"/>
+      <c r="G4" t="s"/>
       <c r="H4" t="s"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s"/>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B5" t="s"/>
+      <c r="C5" t="s"/>
+      <c r="D5" t="s"/>
       <c r="E5" t="s"/>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
+      <c r="F5" t="s"/>
       <c r="G5" t="s"/>
       <c r="H5" t="s"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s"/>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
+      <c r="B6" t="s"/>
+      <c r="C6" t="s"/>
+      <c r="D6" t="s"/>
       <c r="E6" t="s"/>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
+      <c r="F6" t="s"/>
       <c r="G6" t="s"/>
       <c r="H6" t="s"/>
     </row>

</xml_diff>